<commit_message>
back to classes d origine, juste chgt nom des pacakges
</commit_message>
<xml_diff>
--- a/target/test-classes/org/squashtest/tm/plugin/custom/report/segur/generateExcelFilePrepublication.xlsx
+++ b/target/test-classes/org/squashtest/tm/plugin/custom/report/segur/generateExcelFilePrepublication.xlsx
@@ -209,7 +209,9 @@
     <t>PSC.03</t>
   </si>
   <si>
-    <t>texte de l'éxigence avec paragraphes :&lt;/br&gt; &lt;p&gt;P1 : text &lt;/p&gt;&lt;p&gt;P2 : text 2&lt;/p&gt;</t>
+    <t>texte de l'éxigence avec paragraphes :
+P1 : text 
+P2 : text 2</t>
   </si>
   <si>
     <t>Ceci est un autre commentaire</t>
@@ -221,22 +223,21 @@
     <t>INS.01.01</t>
   </si>
   <si>
-    <t>&lt;p&gt;paragraphe&lt;/p&gt;
-&lt;p&gt;ligne 1&lt;br /&gt;
-ligne 2&lt;br /&gt;
-ligne 3&lt;/p&gt;
-&lt;p&gt;paragraphe 1&lt;/p&gt;
-&lt;p&gt;paragraphe 2&lt;/p&gt;
-&lt;p&gt; &lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;résultat attendu avec paragraphe (order 2)  &amp;amp; (ampersand) ou &amp;gt; (supérieur)&lt;BR/&gt;&lt;/p&gt;</t>
+    <t>paragraphe
+ligne 1
+ligne 2
+ligne 3
+paragraphe 1
+paragraphe 2</t>
+  </si>
+  <si>
+    <t>résultat attendu avec paragraphe (order 2)  &amp; (ampersand) ou &gt; (supérieur)</t>
   </si>
   <si>
     <t>INS.01.10</t>
   </si>
   <si>
-    <t>résultat attendu step 2 (order 1)&lt;BR/&gt; &lt;ul&gt;&lt;li&gt;1ere ligne&lt;/li&gt;&lt;li&gt;2eme ligne&lt;/li&gt;&lt;/ul&gt;</t>
+    <t>résultat attendu step 2 (order 1) * 1ere ligne* 2eme ligne</t>
   </si>
   <si>
     <t xml:space="preserve"> </t>
@@ -248,7 +249,7 @@
     <t>SC.INS.01.01</t>
   </si>
   <si>
-    <t>&lt;p&gt;Ceci est une note interne&lt;/p&gt;</t>
+    <t>Ceci est une note interne</t>
   </si>
   <si>
     <t>Remarque Ségur</t>
@@ -257,11 +258,7 @@
     <t>Gestion de l'ins Alimentation du DMP via une PFI</t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;p&gt;
-        Lorsqu&amp;#39;une BAL est bloqu&amp;eacute;e par un administrateur global, des &amp;quot;traces fonctionnelles&amp;quot; et applicatives sont constitu&amp;eacute;es et doivent au moins contenir les informations suivantes :&lt;/p&gt;
-&lt;ul&gt;
-        &lt;li&gt;                type d&amp;#39;action ;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp; &amp;nbsp;&lt;/li&gt;        &lt;li&gt;                identit&amp;eacute; de son auteur ;&lt;/li&gt;        &lt;li&gt;                dates et heures ;&lt;/li&gt;        &lt;li&gt;                moyens techniques utilis&amp;eacute;s (LPS, WPS, etc..) ;&lt;/li&gt;        &lt;li&gt;                adresse r&amp;eacute;seau&lt;/li&gt;        &lt;li&gt;                ...&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;        &amp;nbsp;&lt;/p&gt;
-</t>
+    <t>Lorsqu'une BAL est bloquée par un administrateur global, des "traces fonctionnelles" et applicatives sont constituées et doivent au moins contenir les informations suivantes :        *                 type d'action ;                *                 identité de son auteur ;        *                 dates et heures ;        *                 moyens techniques utilisés (LPS, WPS, etc..) ;        *                 adresse réseau        *                 ...         </t>
   </si>
   <si>
     <t>Ceci est un commentaire</t>
@@ -270,7 +267,10 @@
     <t>Modifiée</t>
   </si>
   <si>
-    <t>&lt;strong&gt;description&lt;/strong&gt; du cas de test sans pré-requis et sans steps avec l&amp;apos;apostrophe&lt;ol start="3"&gt;&lt;li&gt;element ordonné (la liste démarre à 3)&lt;/li&gt;&lt;li&gt;element ordonné ( deuxième élément de la liste : numéro 4)&lt;/li&gt;&lt;/ol&gt;reprise du texte après la liste, il faut Une ligne blanche avant</t>
+    <t>description du cas de test sans pré-requis et sans steps avec l'apostrophe
+3.element ordonné (la liste démarre à 3)
+4.element ordonné ( deuxième élément de la liste : numéro 4)
+reprise du texte après la liste, il faut Une ligne blanche avant</t>
   </si>
   <si>
     <t>REF-2</t>
@@ -298,7 +298,7 @@
     <t>CI-SIS/MSS.02</t>
   </si>
   <si>
-    <t>En cas de modification d'un des documents listés dans le DSR en annexe 3, le système DOIT pouvoir transmettre par messagerie sécurisée de santé la nouvelle version du document avec une mention du type &amp;quot;annule &amp;amp; remplace&amp;quot; pré-paramétrée.</t>
+    <t>En cas de modification d'un des documents listés dans le DSR en annexe 3, le système DOIT pouvoir transmettre par messagerie sécurisée de santé la nouvelle version du document avec une mention du type "annule &amp; remplace" pré-paramétrée.</t>
   </si>
   <si>
     <t>Ceci est encore un autre commentaire</t>

</xml_diff>